<commit_message>
I updated workflow dates for sample preparation (Marie-Amélie Pussacq internship).
</commit_message>
<xml_diff>
--- a/1_data/1_data_nutrient/2_data_samples/faeces_samples.xlsx
+++ b/1_data/1_data_nutrient/2_data_samples/faeces_samples.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3334" uniqueCount="1099">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3338" uniqueCount="1099">
   <si>
     <t xml:space="preserve">sample_type</t>
   </si>
@@ -3489,10 +3489,10 @@
   </sheetPr>
   <dimension ref="A1:S431"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A334" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="D368" activeCellId="0" sqref="D368"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A219" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D236" activeCellId="0" sqref="D236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14736,7 +14736,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="1" t="s">
         <v>19</v>
       </c>
@@ -14764,6 +14764,15 @@
       <c r="I252" s="2" t="s">
         <v>646</v>
       </c>
+      <c r="J252" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="K252" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="L252" s="2" t="s">
+        <v>405</v>
+      </c>
       <c r="P252" s="1" t="s">
         <v>717</v>
       </c>
@@ -19810,6 +19819,9 @@
       </c>
       <c r="K386" s="2" t="s">
         <v>401</v>
+      </c>
+      <c r="L386" s="2" t="s">
+        <v>405</v>
       </c>
       <c r="P386" s="1" t="s">
         <v>989</v>
@@ -21502,7 +21514,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.71"/>

</xml_diff>